<commit_message>
adding some 2022 fcr mom samples
</commit_message>
<xml_diff>
--- a/Summer2019-DataAnalysis/RawData/Zoop_sample_counting_template_2019.xlsx
+++ b/Summer2019-DataAnalysis/RawData/Zoop_sample_counting_template_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heatherwander/Documents/VirginiaTech/research/zooplankton/Summer2019-DataAnalysis/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DACDE15-F7E9-DE4C-8132-C69C526B62D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB1FEA3-50A9-7743-888D-31F6DAAACD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16220" xr2:uid="{3D67C25D-D874-DE45-AEE3-7A59E1B23F3C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="32">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -104,22 +104,34 @@
     <t>1 mL</t>
   </si>
   <si>
-    <t>P. sulcata</t>
-  </si>
-  <si>
-    <t>K. bostoniensis</t>
-  </si>
-  <si>
     <t>Ceriodaphnia</t>
   </si>
   <si>
     <t>Trichocerca</t>
   </si>
   <si>
-    <t>Conochiloides</t>
+    <t>Lepadella</t>
   </si>
   <si>
-    <t>B_pel_10Jul19_sunset_h3_rep2</t>
+    <t>B_pel_24Jul19_sunset_h3_rep3</t>
+  </si>
+  <si>
+    <t>Gastropus</t>
+  </si>
+  <si>
+    <t>Conochilus</t>
+  </si>
+  <si>
+    <t>Calanodia</t>
+  </si>
+  <si>
+    <t>Polyarthra</t>
+  </si>
+  <si>
+    <t>Monostyla</t>
+  </si>
+  <si>
+    <t>Lecane</t>
   </si>
 </sst>
 </file>
@@ -526,7 +538,7 @@
   <dimension ref="A1:I1267"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H101"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,7 +554,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C1"/>
       <c r="G1" s="10"/>
@@ -554,7 +566,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>43656</v>
+        <v>43670</v>
       </c>
       <c r="C2"/>
     </row>
@@ -563,7 +575,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>44950</v>
+        <v>44951</v>
       </c>
       <c r="C3"/>
       <c r="E3" t="s">
@@ -625,13 +637,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="8">
-        <v>1</v>
+        <v>3.3</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>9</v>
@@ -639,12 +651,7 @@
       <c r="E8" s="3">
         <v>1200</v>
       </c>
-      <c r="F8" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="9">
-        <v>0.3</v>
-      </c>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -654,7 +661,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="8">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>9</v>
@@ -667,13 +674,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="8">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>
@@ -682,21 +689,21 @@
         <v>1200</v>
       </c>
       <c r="F10" s="11">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G10" s="10">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="8">
-        <v>1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>9</v>
@@ -704,22 +711,18 @@
       <c r="E11" s="3">
         <v>1200</v>
       </c>
-      <c r="F11" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="G11" s="10">
-        <v>0.3</v>
-      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="8">
-        <v>3.1</v>
+        <v>1.3</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>9</v>
@@ -727,18 +730,22 @@
       <c r="E12" s="3">
         <v>1200</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10"/>
+      <c r="F12" s="11">
+        <v>0.9</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="8">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
@@ -751,13 +758,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="8">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
@@ -765,18 +772,22 @@
       <c r="E14" s="3">
         <v>1200</v>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10"/>
+      <c r="F14" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="8">
-        <v>1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
@@ -784,22 +795,18 @@
       <c r="E15" s="3">
         <v>1200</v>
       </c>
-      <c r="F15" s="11">
-        <v>0.5</v>
-      </c>
-      <c r="G15" s="10">
-        <v>0.3</v>
-      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="8">
-        <v>1.1000000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>9</v>
@@ -807,22 +814,18 @@
       <c r="E16" s="3">
         <v>1200</v>
       </c>
-      <c r="F16" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="G16" s="10">
-        <v>0.6</v>
-      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="10"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="8">
-        <v>1.6</v>
+        <v>1.3</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
@@ -830,22 +833,18 @@
       <c r="E17" s="3">
         <v>1200</v>
       </c>
-      <c r="F17" s="11">
-        <v>0.8</v>
-      </c>
-      <c r="G17" s="10">
-        <v>0.7</v>
-      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="10"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="8">
-        <v>2.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>9</v>
@@ -853,18 +852,22 @@
       <c r="E18" s="3">
         <v>1200</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="10"/>
+      <c r="F18" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="8">
-        <v>1.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>9</v>
@@ -872,18 +875,22 @@
       <c r="E19" s="3">
         <v>1200</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="10"/>
+      <c r="F19" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="8">
-        <v>1.3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>9</v>
@@ -891,18 +898,22 @@
       <c r="E20" s="3">
         <v>1200</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="10"/>
+      <c r="F20" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="8">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>9</v>
@@ -911,10 +922,10 @@
         <v>1200</v>
       </c>
       <c r="F21" s="11">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G21" s="10">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -925,7 +936,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="8">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>9</v>
@@ -938,13 +949,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="8">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>9</v>
@@ -961,13 +972,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="8">
-        <v>1.1000000000000001</v>
+        <v>2.4</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>9</v>
@@ -975,22 +986,18 @@
       <c r="E24" s="3">
         <v>1200</v>
       </c>
-      <c r="F24" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G24" s="10">
-        <v>0.6</v>
-      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="8">
-        <v>1.4</v>
+        <v>0.8</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>9</v>
@@ -998,18 +1005,22 @@
       <c r="E25" s="3">
         <v>1200</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="F25" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="8">
-        <v>1.1000000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>9</v>
@@ -1018,22 +1029,18 @@
         <v>1200</v>
       </c>
       <c r="F26" s="8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G26" s="8">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C27" s="8">
-        <v>6.5</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="3" t="s">
         <v>9</v>
       </c>
@@ -1045,13 +1052,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="8">
-        <v>1.3</v>
+        <v>1.9</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>9</v>
@@ -1059,18 +1066,22 @@
       <c r="E28" s="3">
         <v>1200</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
+      <c r="F28" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="G28" s="8">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="8">
-        <v>2.5</v>
+        <v>3.8</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>9</v>
@@ -1082,7 +1093,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>11</v>
@@ -1097,21 +1108,21 @@
         <v>1200</v>
       </c>
       <c r="F30" s="8">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="G30" s="8">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C31" s="8">
-        <v>1.2</v>
+        <v>6.6</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>9</v>
@@ -1123,16 +1134,16 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C32" s="8">
-        <v>1.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E32" s="3">
         <v>1200</v>
@@ -1141,12 +1152,12 @@
         <v>0.8</v>
       </c>
       <c r="G32" s="8">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>11</v>
@@ -1155,21 +1166,21 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E33" s="3">
         <v>1200</v>
       </c>
       <c r="F33" s="8">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="G33" s="8">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>11</v>
@@ -1178,7 +1189,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E34" s="3">
         <v>1200</v>
@@ -1192,58 +1203,50 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="8">
-        <v>3.3</v>
+        <v>1</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E35" s="3">
         <v>1200</v>
       </c>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
+      <c r="F35" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="8">
-        <v>1.1000000000000001</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
       <c r="D36" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E36" s="3">
         <v>1200</v>
       </c>
-      <c r="F36" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G36" s="8">
-        <v>0.6</v>
-      </c>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="8">
-        <v>6.6</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
       <c r="D37" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E37" s="3">
         <v>1200</v>
@@ -1253,16 +1256,12 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="8">
-        <v>5.5</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
       <c r="D38" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E38" s="3">
         <v>1200</v>
@@ -1272,16 +1271,12 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="8">
-        <v>6.9</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
       <c r="D39" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E39" s="3">
         <v>1200</v>
@@ -1290,16 +1285,12 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="8">
-        <v>2</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
       <c r="D40" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E40" s="3">
         <v>1200</v>
@@ -1309,16 +1300,12 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="8">
-        <v>1.6</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
       <c r="D41" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E41" s="3">
         <v>1200</v>
@@ -1327,16 +1314,12 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="9">
-        <v>5.6</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="9"/>
       <c r="D42" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E42" s="3">
         <v>1200</v>
@@ -1346,12 +1329,12 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="9"/>
       <c r="D43" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E43" s="3">
         <v>1200</v>
@@ -1361,12 +1344,12 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="9"/>
       <c r="D44" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E44" s="3">
         <v>1200</v>
@@ -1376,12 +1359,12 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="9"/>
       <c r="D45" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E45" s="3">
         <v>1200</v>
@@ -1391,12 +1374,12 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="9"/>
       <c r="D46" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E46" s="3">
         <v>1200</v>
@@ -1406,12 +1389,12 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
       <c r="D47" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E47" s="3">
         <v>1200</v>
@@ -1421,96 +1404,104 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="8">
-        <v>6.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E48" s="3">
         <v>1200</v>
       </c>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F48" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G48" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C49" s="8">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E49" s="3">
         <v>1200</v>
       </c>
       <c r="F49" s="8">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="G49" s="8">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C50" s="9">
-        <v>0.9</v>
+        <v>1.4</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E50" s="3">
         <v>1200</v>
       </c>
-      <c r="F50" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G50" s="8">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C51" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="E51" s="3">
         <v>1200</v>
       </c>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F51" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G51" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
+      <c r="B52" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="8">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="D52" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E52" s="3">
         <v>1200</v>
@@ -1518,197 +1509,171 @@
       <c r="F52" s="8"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="8">
-        <v>9.1999999999999993</v>
-      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
       <c r="D53" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E53" s="3">
         <v>1200</v>
       </c>
       <c r="F53" s="8"/>
       <c r="G53" s="8"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C54" s="8">
-        <v>1.1000000000000001</v>
+        <v>6.5</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E54" s="3">
         <v>1200</v>
       </c>
-      <c r="F54" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G54" s="8">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C55" s="8">
-        <v>1.1000000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E55" s="3">
         <v>1200</v>
       </c>
       <c r="F55" s="8">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="G55" s="8">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="9">
-        <v>3.3</v>
+      <c r="C56" s="8">
+        <v>0.9</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E56" s="3">
         <v>1200</v>
       </c>
-      <c r="F56" s="8"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F56" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G56" s="8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" s="9">
-        <v>5.6</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="9"/>
       <c r="D57" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E57" s="3">
         <v>1200</v>
       </c>
       <c r="F57" s="8"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="9">
-        <v>0.8</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B58" s="8"/>
+      <c r="C58" s="9"/>
       <c r="D58" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E58" s="3">
         <v>1200</v>
       </c>
-      <c r="F58" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="G58" s="9">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="9">
-        <v>8.6999999999999993</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="9"/>
       <c r="D59" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E59" s="3">
         <v>1200</v>
       </c>
       <c r="F59" s="8"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60" s="9">
-        <v>1</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="9"/>
       <c r="D60" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E60" s="3">
         <v>1200</v>
       </c>
-      <c r="F60" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="G60" s="9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="9"/>
       <c r="D61" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E61" s="3">
         <v>1200</v>
       </c>
       <c r="F61" s="8"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C62" s="9">
-        <v>6.5</v>
+        <v>2.1</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E62" s="3">
         <v>1200</v>
@@ -1716,47 +1681,56 @@
       <c r="F62" s="8"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C63" s="9">
-        <v>2.9</v>
+        <v>1.3</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E63" s="3">
         <v>1200</v>
       </c>
       <c r="F63" s="8"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B64" s="8"/>
-      <c r="C64" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="9">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="D64" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E64" s="3">
         <v>1200</v>
       </c>
-      <c r="F64" s="8"/>
+      <c r="F64" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="G64" s="9">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C65" s="9">
-        <v>5.4</v>
+        <v>1.4</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>14</v>
@@ -1764,15 +1738,23 @@
       <c r="E65" s="3">
         <v>1200</v>
       </c>
-      <c r="F65" s="8"/>
-      <c r="G65" s="8"/>
+      <c r="F65" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="G65" s="8">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="9"/>
+      <c r="B66" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="9">
+        <v>1.8</v>
+      </c>
       <c r="D66" s="3" t="s">
         <v>14</v>
       </c>
@@ -1783,12 +1765,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B67" s="8"/>
-      <c r="C67" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="9">
+        <v>1.9</v>
+      </c>
       <c r="D67" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E67" s="3">
         <v>1200</v>
@@ -1799,10 +1785,14 @@
       <c r="A68" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="9"/>
+      <c r="B68" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="9">
+        <v>1.5</v>
+      </c>
       <c r="D68" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E68" s="3">
         <v>1200</v>
@@ -1811,73 +1801,81 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C69" s="9">
-        <v>1.1000000000000001</v>
+        <v>2.9</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E69" s="3">
         <v>1200</v>
       </c>
-      <c r="F69" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="G69" s="8">
-        <v>0.6</v>
-      </c>
+      <c r="F69" s="8"/>
+      <c r="G69" s="8"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C70" s="9">
-        <v>5.2</v>
+        <v>0.9</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E70" s="3">
         <v>1200</v>
       </c>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
+      <c r="F70" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G70" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B71" s="8"/>
-      <c r="C71" s="9"/>
+        <v>27</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="9">
+        <v>0.9</v>
+      </c>
       <c r="D71" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E71" s="3">
         <v>1200</v>
       </c>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
+      <c r="F71" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G71" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C72" s="9">
-        <v>6.1</v>
+        <v>1.5</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E72" s="3">
         <v>1200</v>
@@ -1887,12 +1885,16 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B73" s="8"/>
-      <c r="C73" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="9">
+        <v>8.1</v>
+      </c>
       <c r="D73" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E73" s="3">
         <v>1200</v>
@@ -1902,16 +1904,16 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C74" s="9">
-        <v>7.6</v>
+        <v>3.8</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E74" s="3">
         <v>1200</v>
@@ -1920,16 +1922,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C75" s="9">
-        <v>8.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E75" s="3">
         <v>1200</v>
@@ -1938,12 +1940,16 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B76" s="8"/>
-      <c r="C76" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="9">
+        <v>1.5</v>
+      </c>
       <c r="D76" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E76" s="3">
         <v>1200</v>
@@ -1958,29 +1964,33 @@
         <v>11</v>
       </c>
       <c r="C77" s="9">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E77" s="3">
         <v>1200</v>
       </c>
       <c r="F77" s="8">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="G77" s="8">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B78" s="8"/>
-      <c r="C78" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="9">
+        <v>3.2</v>
+      </c>
       <c r="D78" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E78" s="3">
         <v>1200</v>
@@ -1989,30 +1999,39 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C79" s="9">
-        <v>6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E79" s="3">
         <v>1200</v>
       </c>
-      <c r="F79" s="8"/>
+      <c r="F79" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G79" s="9">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" s="9">
+        <v>1.4</v>
+      </c>
       <c r="D80" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E80" s="3">
         <v>1200</v>
@@ -2027,7 +2046,7 @@
       <c r="B81" s="8"/>
       <c r="C81" s="9"/>
       <c r="D81" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E81" s="3">
         <v>1200</v>
@@ -2037,26 +2056,39 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B82" s="8"/>
-      <c r="C82" s="9"/>
+        <v>23</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="9">
+        <v>1.6</v>
+      </c>
       <c r="D82" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E82" s="3">
         <v>1200</v>
       </c>
-      <c r="F82" s="8"/>
+      <c r="F82" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G82" s="9">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B83" s="8"/>
-      <c r="C83" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="9">
+        <v>2.5</v>
+      </c>
       <c r="D83" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E83" s="3">
         <v>1200</v>
@@ -2065,27 +2097,35 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B84" s="8"/>
-      <c r="C84" s="9"/>
+        <v>30</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="9">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="D84" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E84" s="3">
         <v>1200</v>
       </c>
-      <c r="F84" s="8"/>
-      <c r="G84" s="8"/>
+      <c r="F84" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="G84" s="8">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B85" s="8"/>
       <c r="C85" s="8"/>
       <c r="D85" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E85" s="3">
         <v>1200</v>
@@ -2095,17 +2135,26 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" s="8">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="D86" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E86" s="3">
         <v>1200</v>
       </c>
-      <c r="F86" s="8"/>
+      <c r="F86" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="G86" s="9">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
@@ -2114,7 +2163,7 @@
       <c r="B87" s="8"/>
       <c r="C87" s="9"/>
       <c r="D87" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E87" s="3">
         <v>1200</v>
@@ -2123,12 +2172,12 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B88" s="8"/>
       <c r="C88" s="9"/>
       <c r="D88" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E88" s="3">
         <v>1200</v>
@@ -2138,12 +2187,12 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B89" s="8"/>
       <c r="C89" s="9"/>
       <c r="D89" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E89" s="3">
         <v>1200</v>
@@ -2152,12 +2201,12 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B90" s="8"/>
       <c r="C90" s="9"/>
       <c r="D90" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E90" s="3">
         <v>1200</v>
@@ -2166,12 +2215,12 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B91" s="8"/>
       <c r="C91" s="9"/>
       <c r="D91" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E91" s="3">
         <v>1200</v>
@@ -2181,12 +2230,12 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B92" s="8"/>
       <c r="C92" s="9"/>
       <c r="D92" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E92" s="3">
         <v>1200</v>
@@ -2195,12 +2244,12 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="9"/>
       <c r="D93" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E93" s="3">
         <v>1200</v>
@@ -2209,12 +2258,12 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="9"/>
       <c r="D94" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E94" s="3">
         <v>1200</v>
@@ -2224,12 +2273,12 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B95" s="8"/>
       <c r="C95" s="9"/>
       <c r="D95" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E95" s="3">
         <v>1200</v>
@@ -2239,12 +2288,12 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B96" s="8"/>
       <c r="C96" s="9"/>
       <c r="D96" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E96" s="3">
         <v>1200</v>
@@ -2254,12 +2303,12 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B97" s="8"/>
       <c r="C97" s="9"/>
       <c r="D97" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E97" s="3">
         <v>1200</v>
@@ -2269,12 +2318,12 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B98" s="8"/>
       <c r="C98" s="9"/>
       <c r="D98" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E98" s="3">
         <v>1200</v>
@@ -2285,10 +2334,14 @@
       <c r="A99" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B99" s="8"/>
-      <c r="C99" s="9"/>
+      <c r="B99" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" s="9">
+        <v>5.7</v>
+      </c>
       <c r="D99" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E99" s="3">
         <v>1200</v>
@@ -2297,12 +2350,12 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="9"/>
       <c r="D100" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E100" s="3">
         <v>1200</v>
@@ -2312,347 +2365,644 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B101" s="8"/>
       <c r="C101" s="9"/>
       <c r="D101" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E101" s="3">
         <v>1200</v>
       </c>
       <c r="F101" s="8"/>
       <c r="G101" s="8"/>
-      <c r="H101" t="s">
-        <v>20</v>
-      </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="3"/>
-      <c r="B102" s="8"/>
-      <c r="C102" s="9"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
+      <c r="A102" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C102" s="9">
+        <v>5.3</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E102" s="3">
+        <v>1200</v>
+      </c>
       <c r="F102" s="8"/>
       <c r="G102" s="8"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="3"/>
+      <c r="A103" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B103" s="8"/>
       <c r="C103" s="9"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="3"/>
+      <c r="D103" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E103" s="3">
+        <v>1200</v>
+      </c>
       <c r="F103" s="8"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="3"/>
-      <c r="B104" s="8"/>
-      <c r="C104" s="9"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="3"/>
+      <c r="A104" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C104" s="9">
+        <v>1.9</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E104" s="3">
+        <v>1200</v>
+      </c>
       <c r="F104" s="8"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="3"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="9"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
-      <c r="F105" s="8"/>
-      <c r="G105" s="8"/>
+      <c r="A105" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C105" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E105" s="3">
+        <v>1200</v>
+      </c>
+      <c r="F105" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="G105" s="8">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="3"/>
+      <c r="A106" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B106" s="8"/>
       <c r="C106" s="9"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="3"/>
+      <c r="D106" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E106" s="3">
+        <v>1200</v>
+      </c>
       <c r="F106" s="8"/>
       <c r="G106" s="8"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="3"/>
+      <c r="A107" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B107" s="8"/>
       <c r="C107" s="9"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="3"/>
+      <c r="D107" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E107" s="3">
+        <v>1200</v>
+      </c>
       <c r="F107" s="8"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="3"/>
-      <c r="B108" s="8"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="3"/>
+      <c r="A108" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B108" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E108" s="3">
+        <v>1200</v>
+      </c>
       <c r="F108" s="11"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="3"/>
-      <c r="B109" s="8"/>
-      <c r="C109" s="10"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="3"/>
+      <c r="A109" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E109" s="3">
+        <v>1200</v>
+      </c>
       <c r="F109" s="11"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="3"/>
-      <c r="B110" s="8"/>
-      <c r="C110" s="9"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="8"/>
+      <c r="A110" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C110" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E110" s="3">
+        <v>1200</v>
+      </c>
+      <c r="F110" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="G110" s="9">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="3"/>
+      <c r="A111" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="B111" s="8"/>
       <c r="C111" s="10"/>
-      <c r="D111" s="3"/>
-      <c r="E111" s="3"/>
+      <c r="D111" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E111" s="3">
+        <v>1200</v>
+      </c>
       <c r="F111" s="11"/>
+      <c r="H111" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="3"/>
+      <c r="A112" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B112" s="8"/>
       <c r="C112" s="10"/>
-      <c r="D112" s="3"/>
-      <c r="E112" s="3"/>
+      <c r="D112" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E112" s="3">
+        <v>1200</v>
+      </c>
       <c r="F112" s="11"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A113" s="3"/>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B113" s="8"/>
       <c r="C113" s="9"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="3"/>
+      <c r="D113" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E113" s="3">
+        <v>1200</v>
+      </c>
       <c r="F113" s="8"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="3"/>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B114" s="11"/>
       <c r="C114" s="9"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="3"/>
+      <c r="D114" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E114" s="3">
+        <v>1200</v>
+      </c>
       <c r="F114" s="8"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A115" s="3"/>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B115" s="11"/>
       <c r="C115" s="9"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
+      <c r="D115" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E115" s="3">
+        <v>1200</v>
+      </c>
       <c r="F115" s="8"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" s="3"/>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B116" s="11"/>
       <c r="C116" s="9"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
+      <c r="D116" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E116" s="3">
+        <v>1200</v>
+      </c>
       <c r="F116" s="8"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" s="3"/>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B117" s="11"/>
       <c r="C117" s="9"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
+      <c r="D117" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E117" s="3">
+        <v>1200</v>
+      </c>
       <c r="F117" s="8"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A118" s="3"/>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B118" s="8"/>
       <c r="C118" s="9"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
+      <c r="D118" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E118" s="3">
+        <v>1200</v>
+      </c>
       <c r="F118" s="8"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" s="3"/>
-      <c r="B119" s="8"/>
-      <c r="C119" s="9"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E119" s="3">
+        <v>1200</v>
+      </c>
       <c r="F119" s="8"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A120" s="3"/>
-      <c r="B120" s="8"/>
-      <c r="C120" s="9"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3"/>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C120" s="9">
+        <v>1.9</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E120" s="3">
+        <v>1200</v>
+      </c>
       <c r="F120" s="8"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A121" s="3"/>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B121" s="8"/>
       <c r="C121" s="9"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3"/>
+      <c r="D121" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E121" s="3">
+        <v>1200</v>
+      </c>
       <c r="F121" s="8"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A122" s="3"/>
-      <c r="B122" s="8"/>
-      <c r="C122" s="9"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
-      <c r="F122" s="8"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A123" s="3"/>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C122" s="9">
+        <v>1</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E122" s="3">
+        <v>1200</v>
+      </c>
+      <c r="F122" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="G122" s="9">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B123" s="8"/>
       <c r="C123" s="9"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3"/>
+      <c r="D123" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E123" s="3">
+        <v>1200</v>
+      </c>
       <c r="F123" s="8"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A124" s="3"/>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B124" s="8"/>
       <c r="C124" s="9"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
+      <c r="D124" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E124" s="3">
+        <v>1200</v>
+      </c>
       <c r="F124" s="8"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A125" s="3"/>
+      <c r="H124" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B125" s="8"/>
       <c r="C125" s="9"/>
-      <c r="D125" s="3"/>
-      <c r="E125" s="3"/>
+      <c r="D125" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E125" s="3">
+        <v>1200</v>
+      </c>
       <c r="F125" s="8"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A126" s="3"/>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B126" s="8"/>
       <c r="C126" s="9"/>
-      <c r="D126" s="3"/>
-      <c r="E126" s="3"/>
+      <c r="D126" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E126" s="3">
+        <v>1200</v>
+      </c>
       <c r="F126" s="8"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" s="3"/>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B127" s="8"/>
       <c r="C127" s="9"/>
-      <c r="D127" s="3"/>
-      <c r="E127" s="3"/>
+      <c r="D127" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E127" s="3">
+        <v>1200</v>
+      </c>
       <c r="F127" s="8"/>
       <c r="G127" s="8"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" s="3"/>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B128" s="8"/>
       <c r="C128" s="9"/>
-      <c r="D128" s="3"/>
-      <c r="E128" s="3"/>
+      <c r="D128" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E128" s="3">
+        <v>1200</v>
+      </c>
       <c r="F128" s="8"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A129" s="3"/>
+      <c r="A129" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B129" s="8"/>
       <c r="C129" s="9"/>
-      <c r="D129" s="3"/>
-      <c r="E129" s="3"/>
+      <c r="D129" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E129" s="3">
+        <v>1200</v>
+      </c>
       <c r="F129" s="8"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" s="3"/>
+      <c r="A130" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B130" s="8"/>
       <c r="C130" s="9"/>
-      <c r="D130" s="3"/>
-      <c r="E130" s="3"/>
+      <c r="D130" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E130" s="3">
+        <v>1200</v>
+      </c>
       <c r="F130" s="8"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" s="3"/>
+      <c r="A131" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B131" s="8"/>
       <c r="C131" s="9"/>
-      <c r="D131" s="3"/>
-      <c r="E131" s="3"/>
+      <c r="D131" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E131" s="3">
+        <v>1200</v>
+      </c>
       <c r="F131" s="8"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A132" s="3"/>
+      <c r="A132" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B132" s="8"/>
       <c r="C132" s="9"/>
-      <c r="D132" s="3"/>
-      <c r="E132" s="3"/>
+      <c r="D132" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E132" s="3">
+        <v>1200</v>
+      </c>
       <c r="F132" s="8"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A133" s="3"/>
+      <c r="A133" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B133" s="8"/>
       <c r="C133" s="9"/>
-      <c r="D133" s="3"/>
-      <c r="E133" s="3"/>
+      <c r="D133" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E133" s="3">
+        <v>1200</v>
+      </c>
       <c r="F133" s="8"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A134" s="3"/>
+      <c r="A134" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B134" s="8"/>
       <c r="C134" s="9"/>
-      <c r="D134" s="3"/>
-      <c r="E134" s="3"/>
+      <c r="D134" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E134" s="3">
+        <v>1200</v>
+      </c>
       <c r="F134" s="8"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A135" s="3"/>
+      <c r="A135" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="B135" s="8"/>
       <c r="C135" s="9"/>
-      <c r="D135" s="3"/>
-      <c r="E135" s="3"/>
+      <c r="D135" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E135" s="3">
+        <v>1200</v>
+      </c>
       <c r="F135" s="8"/>
       <c r="G135" s="8"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A136" s="3"/>
+      <c r="A136" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B136" s="8"/>
       <c r="C136" s="9"/>
-      <c r="D136" s="3"/>
-      <c r="E136" s="3"/>
+      <c r="D136" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E136" s="3">
+        <v>1200</v>
+      </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A137" s="3"/>
+      <c r="A137" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="B137" s="8"/>
       <c r="C137" s="9"/>
-      <c r="D137" s="3"/>
-      <c r="E137" s="3"/>
+      <c r="D137" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E137" s="3">
+        <v>1200</v>
+      </c>
       <c r="F137" s="8"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A138" s="3"/>
+      <c r="A138" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B138" s="8"/>
       <c r="C138" s="9"/>
-      <c r="D138" s="3"/>
-      <c r="E138" s="3"/>
+      <c r="D138" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E138" s="3">
+        <v>1200</v>
+      </c>
       <c r="F138" s="8"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A139" s="3"/>
+      <c r="A139" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B139" s="8"/>
       <c r="C139" s="9"/>
-      <c r="D139" s="3"/>
-      <c r="E139" s="3"/>
+      <c r="D139" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E139" s="3">
+        <v>1200</v>
+      </c>
       <c r="F139" s="8"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A140" s="3"/>
-      <c r="B140" s="8"/>
-      <c r="C140" s="9"/>
-      <c r="D140" s="3"/>
-      <c r="E140" s="3"/>
+      <c r="A140" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C140" s="9">
+        <v>6.5</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E140" s="3">
+        <v>1200</v>
+      </c>
       <c r="F140" s="8"/>
       <c r="G140" s="8"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A141" s="3"/>
+      <c r="A141" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="B141" s="8"/>
       <c r="C141" s="9"/>
-      <c r="D141" s="3"/>
-      <c r="E141" s="3"/>
+      <c r="D141" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E141" s="3">
+        <v>1200</v>
+      </c>
       <c r="F141" s="8"/>
       <c r="G141" s="8"/>
     </row>

</xml_diff>